<commit_message>
Fixing bugs for 1.2
</commit_message>
<xml_diff>
--- a/test/HWDBUtility/SystemTest/003/Biff_3.xlsx
+++ b/test/HWDBUtility/SystemTest/003/Biff_3.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Biff-Items" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t xml:space="preserve">Record Type</t>
   </si>
@@ -73,22 +74,37 @@
     <t xml:space="preserve">Right Bongo</t>
   </si>
   <si>
+    <t xml:space="preserve">7776665555</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cygnus gas field is a natural gas reservoir and gas production facilities in the UK sector of the southern North Sea. It is about 150 km of east of the Lincolnshire coast and started gas production in 2016. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z00100300023-00110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z00100300023-00111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z00100300022-00061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN-8675309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN-3278576</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN-8664295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Really long Institution Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">new</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z00100300023-00110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z00100300023-00111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z00100300022-00061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SN-8675309</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editing</t>
   </si>
 </sst>
 </file>
@@ -179,29 +195,49 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -229,10 +265,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1048576"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -240,8 +276,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="22.62"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="1" width="8.54"/>
@@ -254,14 +290,14 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -270,14 +306,14 @@
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -286,20 +322,21 @@
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="b">
+      <c r="B4" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C4" s="4"/>
@@ -312,16 +349,16 @@
       <c r="J4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
@@ -355,9 +392,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="n">
-        <v>7776665555</v>
+    <row r="7" customFormat="false" ht="59" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>186</v>
@@ -365,8 +402,8 @@
       <c r="D7" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>17</v>
+      <c r="E7" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>96.83</v>
@@ -378,40 +415,84 @@
         <v>111.28</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>100.01</v>
       </c>
-      <c r="G8" s="7" t="n">
+      <c r="G8" s="8" t="n">
         <v>100</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>99.99</v>
       </c>
-      <c r="I8" s="0"/>
-    </row>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="A5:J5"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -420,4 +501,197 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="37.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="14.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="16.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="26.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="10" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="10" width="22.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="10" width="8.54"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="10" t="n">
+        <v>7776665555</v>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>186</v>
+      </c>
+      <c r="D7" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="10" t="n">
+        <v>96.83</v>
+      </c>
+      <c r="G7" s="10" t="n">
+        <v>100.84</v>
+      </c>
+      <c r="H7" s="10" t="n">
+        <v>111.28</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="10" t="n">
+        <v>100.01</v>
+      </c>
+      <c r="G8" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="H8" s="10" t="n">
+        <v>99.99</v>
+      </c>
+      <c r="I8" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>